<commit_message>
Reevaluate with optimal K
</commit_message>
<xml_diff>
--- a/Analyse.xlsx
+++ b/Analyse.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="grid_search" localSheetId="0">Feuil1!$D$3:$E$9</definedName>
-    <definedName name="grid_search_1" localSheetId="0">Feuil1!$D$16:$E$17</definedName>
+    <definedName name="grid_search" localSheetId="0">Feuil1!$E$3:$F$9</definedName>
+    <definedName name="grid_search_1" localSheetId="0">Feuil1!$E$16:$F$17</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>K</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Dataset</t>
+  </si>
+  <si>
+    <t>Zero neigh.</t>
+  </si>
+  <si>
+    <t>K = 60</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -163,6 +169,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="171" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -194,6 +206,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Recherche</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> du paramètre K optimal</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -247,7 +289,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$D$3:$D$17</c:f>
+              <c:f>Feuil1!$E$3:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -301,7 +343,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$E$3:$E$17</c:f>
+              <c:f>Feuil1!$F$3:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -374,6 +416,81 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>K</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> : Nombre de voisins à considérer</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -439,6 +556,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Qualité</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> MAE</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -481,38 +659,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1110,13 +1256,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>6350</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -1412,202 +1558,231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="5" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D1" s="6" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="9"/>
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="7">
+        <v>0.76612471040799301</v>
+      </c>
+      <c r="C3" s="5">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2">
         <v>0.77604501622557298</v>
       </c>
-      <c r="D3" s="5">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.77604501622557298</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>0.77237816086820199</v>
-      </c>
-      <c r="D4" s="5">
+        <v>0.76093146583641302</v>
+      </c>
+      <c r="C4" s="5">
+        <v>36</v>
+      </c>
+      <c r="E4" s="5">
         <v>25</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0.77332987647696905</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="7">
-        <v>0.76636818676071305</v>
-      </c>
-      <c r="D5" s="5">
+        <v>0.75366757154961606</v>
+      </c>
+      <c r="C5" s="5">
+        <v>36</v>
+      </c>
+      <c r="E5" s="5">
         <v>30</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>0.77133156480005904</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="7">
-        <v>0.76320455950684396</v>
-      </c>
-      <c r="D6" s="5">
+        <v>0.75232821263713801</v>
+      </c>
+      <c r="C6" s="5">
+        <v>27</v>
+      </c>
+      <c r="E6" s="5">
         <v>35</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>0.76962414648157895</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>0.76535964312861404</v>
-      </c>
-      <c r="D7" s="5">
+        <v>0.75763373521216404</v>
+      </c>
+      <c r="C7" s="5">
+        <v>36</v>
+      </c>
+      <c r="E7" s="5">
         <v>40</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>0.76851529993202805</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="8">
         <f>AVERAGE(B3:B7)</f>
-        <v>0.76867111329798921</v>
-      </c>
-      <c r="D8" s="5">
+        <v>0.75813713912866487</v>
+      </c>
+      <c r="C8" s="10">
+        <f>AVERAGE(C3:C7)</f>
+        <v>33.4</v>
+      </c>
+      <c r="E8" s="5">
         <v>45</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>0.76740947383817304</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D9" s="5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E9" s="5">
         <v>50</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>0.76685423988771595</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D10" s="5">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" s="5">
         <v>55</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.76623837245506499</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D11" s="5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11" s="5">
         <v>60</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.76612471040799301</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D12" s="5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="5">
         <v>65</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>0.76612141043604898</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D13" s="5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13" s="5">
         <v>70</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>0.76614362826035198</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D14" s="5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" s="5">
         <v>75</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>0.76625369981790303</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D15" s="5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="5">
         <v>80</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>0.76625197940009604</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D16" s="5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16" s="5">
         <v>85</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>0.76626289000937697</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D17" s="5">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E17" s="5">
         <v>90</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>0.76642400541852296</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
+  <mergeCells count="2">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E8:E15">
+  <conditionalFormatting sqref="F8:F15">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1619,7 +1794,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E15">
+  <conditionalFormatting sqref="F5:F15">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1631,7 +1806,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E17">
+  <conditionalFormatting sqref="F3:F17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>